<commit_message>
add file for importing CSR system fil
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
+++ b/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="3040" yWindow="180" windowWidth="25920" windowHeight="12200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
-    <t>Parameter</t>
-  </si>
-  <si>
     <t>Spectrometer serial number</t>
   </si>
   <si>
@@ -37,9 +34,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>JAZ</t>
@@ -74,12 +68,6 @@
     <t>Spectrometer System Name</t>
   </si>
   <si>
-    <t>UCD_WUEoptimized_Channel1</t>
-  </si>
-  <si>
-    <t>UCD_WUEoptimized_Channel2</t>
-  </si>
-  <si>
     <t>Longpass filter [nm]</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
   </si>
   <si>
     <t>30,40,40,40,60,30</t>
-  </si>
-  <si>
-    <t>Tyson's comments</t>
   </si>
   <si>
     <t>Reference (barium sulfate, foam core, spectralon NIST)</t>
@@ -108,19 +93,52 @@
   <si>
     <t>[If there is a second spectrometer used in this System (as at UNL) info about that can go here]</t>
     <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>UCD_WUEoptimized_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Channel1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>UCD_WUEoptimized_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Channel2</t>
+    </r>
+  </si>
+  <si>
+    <t>Second-spectrometer serial number</t>
+  </si>
+  <si>
+    <t>Parameter_Name</t>
+  </si>
+  <si>
+    <t>Parameter_Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -172,9 +190,17 @@
     <font>
       <sz val="12"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -195,7 +221,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="9"/>
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,7 +246,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,7 +265,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -244,7 +275,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -585,175 +629,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
-    <col min="2" max="3" width="32.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="106.5" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="93.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="18" customFormat="1">
+      <c r="A2" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+    </row>
+    <row r="3" spans="1:5" s="18" customFormat="1">
+      <c r="A3" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="15"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="18" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="18" customFormat="1">
+      <c r="A4" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="18" customFormat="1">
+      <c r="A5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="15"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>14</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="5">
-        <v>590</v>
-      </c>
-      <c r="C7" s="5">
-        <v>660</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" s="5">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5"/>
+        <v>590</v>
+      </c>
+      <c r="C8" s="5">
+        <v>660</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="8"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>18</v>
       </c>
       <c r="C12" s="6"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:5">
-      <c r="B14"/>
-      <c r="C14"/>
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="B15"/>
       <c r="C15"/>
-      <c r="D15"/>
     </row>
     <row r="16" spans="1:5">
       <c r="B16"/>
       <c r="C16"/>
+      <c r="D16"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="12"/>
       <c r="B17"/>
       <c r="C17"/>
     </row>
     <row r="18" spans="1:3">
+      <c r="A18" s="11"/>
       <c r="B18"/>
       <c r="C18"/>
     </row>
@@ -768,6 +815,10 @@
     <row r="21" spans="1:3">
       <c r="B21"/>
       <c r="C21"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="B22"/>
+      <c r="C22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
update CSR system template
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
+++ b/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="0" windowWidth="20740" windowHeight="11760" tabRatio="500"/>
+    <workbookView xWindow="880" yWindow="440" windowWidth="25920" windowHeight="12200" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
-  <si>
-    <t>Parameter</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Spectrometer serial number</t>
   </si>
@@ -37,9 +34,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Comment</t>
   </si>
   <si>
     <t>JAZ</t>
@@ -74,12 +68,6 @@
     <t>Spectrometer System Name</t>
   </si>
   <si>
-    <t>UCD_WUEoptimized_Channel1</t>
-  </si>
-  <si>
-    <t>UCD_WUEoptimized_Channel2</t>
-  </si>
-  <si>
     <t>Longpass filter [nm]</t>
   </si>
   <si>
@@ -93,9 +81,6 @@
   </si>
   <si>
     <t>30,40,40,40,60,30</t>
-  </si>
-  <si>
-    <t>Tyson's comments</t>
   </si>
   <si>
     <t>Reference (barium sulfate, foam core, spectralon NIST)</t>
@@ -106,21 +91,38 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
+    <r>
+      <t>UCD_WUEoptimized_</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Channel1</t>
+    </r>
+  </si>
+  <si>
+    <t>Second-spectrometer serial number</t>
+  </si>
+  <si>
+    <t>Parameter_Name</t>
+  </si>
+  <si>
+    <t>Parameter_Value</t>
+  </si>
+  <si>
     <t>[If there is a second spectrometer used in this System (as at UNL) info about that can go here]</t>
-    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="8">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +157,7 @@
     <font>
       <sz val="8"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -171,10 +174,13 @@
     </font>
     <font>
       <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -193,12 +199,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -209,12 +209,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -233,10 +235,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -244,17 +242,17 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -584,196 +582,173 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:E21"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
-    <col min="2" max="3" width="32.6640625" style="4" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="12" customWidth="1"/>
-    <col min="5" max="5" width="106.5" customWidth="1"/>
+    <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="93.6640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2"/>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B4" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
+      <c r="C4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="5">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B12" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="7"/>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="E3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="5">
-        <v>14</v>
-      </c>
-      <c r="C5" s="5"/>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="5"/>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="5">
-        <v>590</v>
-      </c>
-      <c r="C7" s="5">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="2" t="s">
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
-        <v>10</v>
-      </c>
-      <c r="C8" s="5"/>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="5"/>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="6"/>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="6"/>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="B14"/>
-      <c r="C14"/>
-    </row>
-    <row r="15" spans="1:5">
+    </row>
+    <row r="15" spans="1:4">
       <c r="B15"/>
-      <c r="C15"/>
-      <c r="D15"/>
-    </row>
-    <row r="16" spans="1:5">
+    </row>
+    <row r="16" spans="1:4">
       <c r="B16"/>
       <c r="C16"/>
     </row>
-    <row r="17" spans="1:3">
-      <c r="A17" s="12"/>
+    <row r="17" spans="1:2">
       <c r="B17"/>
-      <c r="C17"/>
-    </row>
-    <row r="18" spans="1:3">
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="10"/>
       <c r="B18"/>
-      <c r="C18"/>
-    </row>
-    <row r="19" spans="1:3">
+    </row>
+    <row r="19" spans="1:2">
       <c r="B19"/>
-      <c r="C19"/>
-    </row>
-    <row r="20" spans="1:3">
+    </row>
+    <row r="20" spans="1:2">
       <c r="B20"/>
-      <c r="C20"/>
-    </row>
-    <row r="21" spans="1:3">
+    </row>
+    <row r="21" spans="1:2">
       <c r="B21"/>
-      <c r="C21"/>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
update Spectrometer System template to use text format for cells instead of general
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
+++ b/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Spectrometer serial number</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Second-spectrometer serial number</t>
-  </si>
-  <si>
-    <t>Parameter_Name</t>
   </si>
   <si>
     <t>Parameter_Value</t>
@@ -216,7 +213,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -229,20 +226,24 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -591,18 +592,18 @@
   <cols>
     <col min="1" max="1" width="46.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="93.6640625" style="10" customWidth="1"/>
+    <col min="3" max="3" width="93.6640625" style="7" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -610,7 +611,7 @@
       <c r="A2" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>22</v>
       </c>
       <c r="C2"/>
@@ -619,7 +620,7 @@
       <c r="A3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
       <c r="C3"/>
@@ -631,7 +632,7 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>6</v>
       </c>
       <c r="C4"/>
@@ -640,16 +641,16 @@
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5"/>
+      <c r="B5" s="13"/>
       <c r="C5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="9">
         <v>14</v>
       </c>
     </row>
@@ -657,7 +658,7 @@
       <c r="A7" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="9" t="s">
         <v>7</v>
       </c>
     </row>
@@ -665,7 +666,7 @@
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="9">
         <v>590</v>
       </c>
     </row>
@@ -681,7 +682,7 @@
       <c r="A10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -689,7 +690,7 @@
       <c r="A11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="9" t="s">
         <v>9</v>
       </c>
     </row>
@@ -697,7 +698,7 @@
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -705,7 +706,7 @@
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="10" t="s">
         <v>19</v>
       </c>
     </row>
@@ -713,7 +714,7 @@
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -728,7 +729,7 @@
       <c r="B17"/>
     </row>
     <row r="18" spans="1:2">
-      <c r="A18" s="10"/>
+      <c r="A18" s="7"/>
       <c r="B18"/>
     </row>
     <row r="19" spans="1:2">

</xml_diff>

<commit_message>
fix link on page and correct error in template for CSR System file
</commit_message>
<xml_diff>
--- a/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
+++ b/curator_data/examples/T3/CSRinT3_SpectrometerSystem.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Spectrometer serial number</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>[If there is a second spectrometer used in this System (as at UNL) info about that can go here]</t>
+  </si>
+  <si>
+    <t>Parameter_Name</t>
   </si>
 </sst>
 </file>
@@ -586,7 +589,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -597,8 +602,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1">
-        <v>3</v>
+      <c r="A1" s="1" t="s">
+        <v>26</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>24</v>

</xml_diff>